<commit_message>
correcoes nas extensões das imagens de jpeg para jpg e ajuste de nomes de arquivos conforme planilha atualizada.
</commit_message>
<xml_diff>
--- a/VEICULOS/112/VEÍCULOS 1.12.xlsx
+++ b/VEICULOS/112/VEÍCULOS 1.12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sesisenaisp.sharepoint.com/sites/GIS/Documentos Compartilhados/Supervisão de Infraestrutura/VEÍCULOS SENAI-SP/VEÍCULOS DIDÁTICOS/112/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sesisenaisp-my.sharepoint.com/personal/jacunda_sp_senai_br/Documents/SENAI/VEICULOS/112/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="11_AD4D361C20488DEA4E38A0613C5D48A65BDEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D869A4E-05BD-4EF5-B043-4E80FA61D706}"/>
+  <xr:revisionPtr revIDLastSave="167" documentId="11_AD4D361C20488DEA4E38A0613C5D48A65BDEDD9F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98FA6D22-273E-45DF-8009-61A0686CBBDB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,9 +140,6 @@
     <t xml:space="preserve">FREEMONT </t>
   </si>
   <si>
-    <t>3C48FABBOCT507036</t>
-  </si>
-  <si>
     <t>IDEA 1.4</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>9C6RG3120G0000001</t>
+  </si>
+  <si>
+    <t>3C4PFABB0CT507036</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1217,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1449,7 +1449,7 @@
         <v>1236477</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>31</v>
@@ -1469,7 +1469,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>14</v>
@@ -1481,7 +1481,7 @@
         <v>1236480</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>31</v>
@@ -1501,7 +1501,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>14</v>
@@ -1513,7 +1513,7 @@
         <v>1236475</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>31</v>
@@ -1533,19 +1533,19 @@
         <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="G10" s="3">
         <v>1362054</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>31</v>
@@ -1565,19 +1565,19 @@
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="G11" s="3">
         <v>1362153</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>31</v>
@@ -1591,16 +1591,16 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>45</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>46</v>
       </c>
       <c r="F12" s="15">
         <v>2002</v>
@@ -1609,7 +1609,7 @@
         <v>1188949</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>31</v>
@@ -1621,16 +1621,16 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="F13" s="15">
         <v>2015</v>
@@ -1639,13 +1639,13 @@
         <v>21</v>
       </c>
       <c r="H13" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1653,16 +1653,16 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="15">
         <v>2015</v>
@@ -1671,13 +1671,13 @@
         <v>21</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -1685,16 +1685,16 @@
         <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F15" s="15">
         <v>2016</v>
@@ -1703,7 +1703,7 @@
         <v>1280818</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>31</v>
@@ -1715,16 +1715,16 @@
         <v>10</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F16" s="15">
         <v>2015</v>
@@ -1733,13 +1733,13 @@
         <v>21</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1751,6 +1751,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Respons_x00e1_vel xmlns="425d0356-a467-47ad-a06b-1c1d23871b07">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Respons_x00e1_vel>
+    <Observa_x00e7__x00f5_es xmlns="425d0356-a467-47ad-a06b-1c1d23871b07" xsi:nil="true"/>
+    <Processo xmlns="425d0356-a467-47ad-a06b-1c1d23871b07" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="425d0356-a467-47ad-a06b-1c1d23871b07">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Status xmlns="425d0356-a467-47ad-a06b-1c1d23871b07">A Fazer</Status>
+    <TaxCatchAll xmlns="4c2b8f09-a594-4c9e-9ecb-2577c1a175a0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010016B08B431EBD4347A48C5FBF37E0FA13" ma:contentTypeVersion="20" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="d7f3a5baaffe486ea196cf167bd31787">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="425d0356-a467-47ad-a06b-1c1d23871b07" xmlns:ns3="4c2b8f09-a594-4c9e-9ecb-2577c1a175a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6cf6643ed0b8086057b4748543ffeaf3" ns2:_="" ns3:_="">
     <xsd:import namespace="425d0356-a467-47ad-a06b-1c1d23871b07"/>
@@ -2038,27 +2059,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Respons_x00e1_vel xmlns="425d0356-a467-47ad-a06b-1c1d23871b07">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Respons_x00e1_vel>
-    <Observa_x00e7__x00f5_es xmlns="425d0356-a467-47ad-a06b-1c1d23871b07" xsi:nil="true"/>
-    <Processo xmlns="425d0356-a467-47ad-a06b-1c1d23871b07" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="425d0356-a467-47ad-a06b-1c1d23871b07">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Status xmlns="425d0356-a467-47ad-a06b-1c1d23871b07">A Fazer</Status>
-    <TaxCatchAll xmlns="4c2b8f09-a594-4c9e-9ecb-2577c1a175a0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2069,6 +2069,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CB1B53B-6E6B-47A4-A36B-20EB12740925}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="425d0356-a467-47ad-a06b-1c1d23871b07"/>
+    <ds:schemaRef ds:uri="4c2b8f09-a594-4c9e-9ecb-2577c1a175a0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A44BF4C-233F-459B-A2A6-A316C85C6C36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2087,17 +2098,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CB1B53B-6E6B-47A4-A36B-20EB12740925}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="425d0356-a467-47ad-a06b-1c1d23871b07"/>
-    <ds:schemaRef ds:uri="4c2b8f09-a594-4c9e-9ecb-2577c1a175a0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF23088-D6A9-4A2A-BC52-22D52DDE7708}">
   <ds:schemaRefs>

</xml_diff>